<commit_message>
Primera version para revision de indra 1.1
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-AppointmentAtenderLE.xlsx
+++ b/docs/StructureDefinition-AppointmentAtenderLE.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-25T12:03:32-03:00</t>
+    <t>2023-01-25T13:45:37-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -7073,7 +7073,7 @@
         <v>85</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I46" t="s" s="2">
         <v>75</v>

</xml_diff>